<commit_message>
bug: attribute schemaname tolower fixed
</commit_message>
<xml_diff>
--- a/FieldCreator/Templates/FieldCreator_Template.xlsx
+++ b/FieldCreator/Templates/FieldCreator_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/ty_corcoran_gapac_com/Documents/Desktop/Work/1_Dev/C#/Projects/XrmToolBox/Field Creator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/ty_corcoran_gapac_com/Documents/Desktop/Work/1_Dev/C#/Projects/XrmToolBox_FieldCreator/Priv/FieldCreator/FieldCreator/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{399127AF-E7BE-441C-AA00-D87F33C41B46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C99656F4-6B4D-47E5-9980-9EACA1151006}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{399127AF-E7BE-441C-AA00-D87F33C41B46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{421CF09F-92A2-4707-99B5-6A6723F06BE9}"/>
   <bookViews>
-    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
   <si>
     <t>Field Type</t>
   </si>
@@ -293,6 +293,24 @@
     </r>
   </si>
   <si>
+    <t>Non-required; Please note character limit in tooltip</t>
+  </si>
+  <si>
+    <t>Non-required; Default is 2</t>
+  </si>
+  <si>
+    <t>Non-required</t>
+  </si>
+  <si>
+    <t>Required for Field Type "Option Set"</t>
+  </si>
+  <si>
+    <t>Required for New Global Option Set type</t>
+  </si>
+  <si>
+    <t>Required for lookups; Must be schema name of entity</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -308,55 +326,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">; 
-</t>
+      <t xml:space="preserve">; </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>*Please note that solution schema name is case-sensitive.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Non-required; Please note character limit in tooltip</t>
-  </si>
-  <si>
-    <t>Non-required; Default is 2</t>
-  </si>
-  <si>
-    <t>Non-required</t>
-  </si>
-  <si>
-    <t>Required for Field Type "Option Set"</t>
-  </si>
-  <si>
-    <t>Required for New Global Option Set type</t>
-  </si>
-  <si>
-    <t>Required for Existing Global Option Set type</t>
-  </si>
-  <si>
-    <t>Required for lookups; Must be schema name of entity</t>
+  </si>
+  <si>
+    <t>Required for New Global Option Set type (must be lowercase)</t>
+  </si>
+  <si>
+    <t>Required for Existing Global Option Set type (must be lowercase)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -373,13 +357,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -786,31 +763,31 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.21875" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.21875" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.7109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -907,7 +884,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -930,7 +907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -953,7 +930,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -982,7 +959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +988,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1043,7 +1020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1049,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1098,7 +1075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1218,23 +1195,21 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.21875" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="22"/>
+    <col min="1" max="1" width="36.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>73</v>
       </c>
@@ -1250,7 +1225,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
@@ -1258,7 +1233,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
@@ -1266,7 +1241,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
@@ -1274,124 +1249,124 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1407,14 +1382,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1422,7 +1397,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1433,7 +1408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1465,7 +1440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1476,7 +1451,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1484,7 +1459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
allow min/max columns to apply to decimals and integers
</commit_message>
<xml_diff>
--- a/FieldCreator/Templates/FieldCreator_Template.xlsx
+++ b/FieldCreator/Templates/FieldCreator_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kochind-my.sharepoint.com/personal/ty_corcoran_gapac_com/Documents/Desktop/Work/1_Dev/C#/Projects/XrmToolBox_FieldCreator/Priv/FieldCreator/FieldCreator/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\xtb\FieldCreator\FieldCreator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{399127AF-E7BE-441C-AA00-D87F33C41B46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{421CF09F-92A2-4707-99B5-6A6723F06BE9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EBC956-C9F8-4BF3-A10A-4DB103029B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Field Type</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>Required for Existing Global Option Set type (must be lowercase)</t>
+  </si>
+  <si>
+    <t>Max Value (Number)</t>
+  </si>
+  <si>
+    <t>Min Value (Number)</t>
   </si>
 </sst>
 </file>
@@ -384,28 +390,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -446,8 +434,8 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Audit Enabled"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Max Length (Single Line of Text)"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Max Length (Multiple Lines of Text)"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Max Value (Whole Number)"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Min Value (Whole Number)"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Max Value (Number)"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Min Value (Number)"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Precision"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Option Set Type"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Option Set Values"/>
@@ -462,9 +450,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +490,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -608,7 +596,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,7 +738,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -761,33 +749,35 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,10 +809,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -849,258 +839,258 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="2">
         <v>523</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="2">
         <v>5000</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="2">
         <v>1000</v>
       </c>
     </row>
@@ -1197,175 +1187,175 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="22"/>
+    <col min="1" max="1" width="36.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1382,14 +1372,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1440,7 +1430,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1451,7 +1441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1459,7 +1449,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>

</xml_diff>